<commit_message>
Amazon page locaters and test added
</commit_message>
<xml_diff>
--- a/target/test-classes/codes_links.xlsx
+++ b/target/test-classes/codes_links.xlsx
@@ -20,12 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t xml:space="preserve">PROMO CODE</t>
   </si>
   <si>
     <t xml:space="preserve">AMAZON LINK</t>
+  </si>
+  <si>
+    <t>75E5GYPF</t>
+  </si>
+  <si>
+    <t>https://amzn.to/35YdcNT</t>
+  </si>
+  <si>
+    <t>50G2LSZS</t>
+  </si>
+  <si>
+    <t>https://amzn.to/34SCPk3</t>
+  </si>
+  <si>
+    <t>70P4RNKQ</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2Gu3zOo</t>
+  </si>
+  <si>
+    <t>OL6CWTAS</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3mOq1RU</t>
+  </si>
+  <si>
+    <t>40G5YMUV</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3oMekN4</t>
+  </si>
+  <si>
+    <t>5NJ7BSJG</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3kQbTa8</t>
+  </si>
+  <si>
+    <t>69226XKI</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2GphbKL</t>
+  </si>
+  <si>
+    <t>5049YPD2</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3enAIYD</t>
   </si>
 </sst>
 </file>
@@ -209,9 +257,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="22.86" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="36.99" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="14.43" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,51 +271,51 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>1</v>
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>1</v>
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
+      <c r="A7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>